<commit_message>
Add Total Column and update show records.
</commit_message>
<xml_diff>
--- a/trading_book.xlsx
+++ b/trading_book.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,6 +464,11 @@
           <t>Notes</t>
         </is>
       </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>Total</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -492,6 +497,7 @@
           <t>EMA</t>
         </is>
       </c>
+      <c r="G2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -519,6 +525,69 @@
         <is>
           <t>SAR EMA MACD</t>
         </is>
+      </c>
+      <c r="G3" t="inlineStr"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1402-05-05</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>BTCUSDT</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D4" t="n">
+        <v>5e-06</v>
+      </c>
+      <c r="E4" t="n">
+        <v>500000</v>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>LW Strategy</t>
+        </is>
+      </c>
+      <c r="G4" t="n">
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1404-01-01</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>ETHUSDT</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SELL</t>
+        </is>
+      </c>
+      <c r="D5" t="n">
+        <v>0.0002</v>
+      </c>
+      <c r="E5" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>Note</t>
+        </is>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fix Errors and Add Export to pdf
</commit_message>
<xml_diff>
--- a/trading_book.xlsx
+++ b/trading_book.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,7 +525,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>SAR EMA MACD</t>
+          <t>SAR EMA MAC</t>
         </is>
       </c>
       <c r="G3" t="n">
@@ -650,7 +650,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>USDTIRT</t>
+          <t>USDT/IRT</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -675,7 +675,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>USDTIRT</t>
+          <t>USDT/IRT</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -689,9 +689,42 @@
       <c r="E9" t="n">
         <v>1.5</v>
       </c>
-      <c r="F9" t="inlineStr"/>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>nan</t>
+        </is>
+      </c>
       <c r="G9" t="n">
         <v>1.5</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="n">
+        <v>45832</v>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>AAVE/USDT</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>Buy</t>
+        </is>
+      </c>
+      <c r="D10" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="E10" t="n">
+        <v>261.18</v>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>T</t>
+        </is>
+      </c>
+      <c r="G10" t="n">
+        <v>5.2236</v>
       </c>
     </row>
   </sheetData>

</xml_diff>